<commit_message>
Update status meeting minute 2
</commit_message>
<xml_diff>
--- a/Meeting Minutes/2.xlsx
+++ b/Meeting Minutes/2.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chung/Documents/webenterprise/Meeting Minutes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\Greenwich\Web Enterprise\Project\Meeting Minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14595" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>ChungNT</t>
   </si>
@@ -92,12 +92,15 @@
   </si>
   <si>
     <t>Sprint Planning</t>
+  </si>
+  <si>
+    <t>Design DB Diagram</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -155,6 +158,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -426,18 +432,18 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="28.83203125" customWidth="1"/>
-    <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.375" customWidth="1"/>
+    <col min="2" max="2" width="28.875" customWidth="1"/>
+    <col min="3" max="3" width="22.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -451,7 +457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -465,13 +471,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -482,7 +493,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -493,7 +504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -504,30 +515,30 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>

</xml_diff>